<commit_message>
added csv for Bergamo
</commit_message>
<xml_diff>
--- a/opendata/it-bergamo-deaths-03.xlsx
+++ b/opendata/it-bergamo-deaths-03.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="268">
   <si>
     <t xml:space="preserve">Provincia di Bergamo</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t xml:space="preserve">Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pop</t>
   </si>
   <si>
     <t xml:space="preserve">Ufficiali Covid</t>
@@ -1233,13 +1236,13 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="11.11"/>
@@ -1262,9 +1265,8 @@
       <c r="D1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="12" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="E1" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="F1" s="13" t="n">
         <v>43525</v>
@@ -1273,7 +1275,7 @@
         <v>43891</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1281,13 +1283,13 @@
         <v>16001</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" s="15" t="n">
         <v>2171</v>
@@ -1302,13 +1304,13 @@
         <v>16002</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E3" s="15" t="n">
         <v>857</v>
@@ -1332,13 +1334,13 @@
         <v>16003</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="15" t="n">
         <v>8075</v>
@@ -1353,13 +1355,13 @@
         <v>16004</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="15" t="n">
         <v>18186</v>
@@ -1383,13 +1385,13 @@
         <v>16248</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="15" t="n">
         <v>726</v>
@@ -1404,13 +1406,13 @@
         <v>16005</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" s="15" t="n">
         <v>5736</v>
@@ -1425,13 +1427,13 @@
         <v>16006</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" s="15" t="n">
         <v>6018</v>
@@ -1455,13 +1457,13 @@
         <v>16007</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E9" s="15" t="n">
         <v>5825</v>
@@ -1476,13 +1478,13 @@
         <v>16008</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" s="15" t="n">
         <v>13757</v>
@@ -1506,13 +1508,13 @@
         <v>16009</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E11" s="15" t="n">
         <v>2343</v>
@@ -1527,13 +1529,13 @@
         <v>16010</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12" s="15" t="n">
         <v>3194</v>
@@ -1548,13 +1550,13 @@
         <v>16011</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E13" s="15" t="n">
         <v>4774</v>
@@ -1569,13 +1571,13 @@
         <v>16012</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E14" s="15" t="n">
         <v>3651</v>
@@ -1590,13 +1592,13 @@
         <v>16013</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E15" s="15" t="n">
         <v>2811</v>
@@ -1611,13 +1613,13 @@
         <v>16014</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E16" s="15" t="n">
         <v>185</v>
@@ -1632,13 +1634,13 @@
         <v>16015</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E17" s="15" t="n">
         <v>525</v>
@@ -1653,13 +1655,13 @@
         <v>16016</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E18" s="15" t="n">
         <v>7685</v>
@@ -1683,13 +1685,13 @@
         <v>16017</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E19" s="15" t="n">
         <v>437</v>
@@ -1713,13 +1715,13 @@
         <v>16018</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E20" s="15" t="n">
         <v>4190</v>
@@ -1743,13 +1745,13 @@
         <v>16019</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E21" s="15" t="n">
         <v>743</v>
@@ -1773,13 +1775,13 @@
         <v>16020</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E22" s="15" t="n">
         <v>4431</v>
@@ -1794,13 +1796,13 @@
         <v>16021</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E23" s="15" t="n">
         <v>1769</v>
@@ -1815,13 +1817,13 @@
         <v>16022</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E24" s="15" t="n">
         <v>734</v>
@@ -1845,13 +1847,13 @@
         <v>16023</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E25" s="15" t="n">
         <v>2492</v>
@@ -1875,13 +1877,13 @@
         <v>16024</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E26" s="15" t="n">
         <v>119551</v>
@@ -1905,13 +1907,13 @@
         <v>16025</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E27" s="15" t="n">
         <v>1309</v>
@@ -1926,13 +1928,13 @@
         <v>16026</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E28" s="15" t="n">
         <v>604</v>
@@ -1956,13 +1958,13 @@
         <v>16027</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E29" s="15" t="n">
         <v>79</v>
@@ -1977,13 +1979,13 @@
         <v>16028</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E30" s="15" t="n">
         <v>5698</v>
@@ -1998,13 +2000,13 @@
         <v>16029</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E31" s="15" t="n">
         <v>5757</v>
@@ -2019,13 +2021,13 @@
         <v>16030</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E32" s="15" t="n">
         <v>8964</v>
@@ -2040,13 +2042,13 @@
         <v>16031</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E33" s="15" t="n">
         <v>6606</v>
@@ -2070,13 +2072,13 @@
         <v>16032</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E34" s="15" t="n">
         <v>1134</v>
@@ -2091,13 +2093,13 @@
         <v>16033</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E35" s="15" t="n">
         <v>977</v>
@@ -2121,13 +2123,13 @@
         <v>16034</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E36" s="15" t="n">
         <v>5254</v>
@@ -2142,13 +2144,13 @@
         <v>16035</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E37" s="15" t="n">
         <v>767</v>
@@ -2172,13 +2174,13 @@
         <v>16036</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E38" s="15" t="n">
         <v>727</v>
@@ -2193,13 +2195,13 @@
         <v>16037</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E39" s="15" t="n">
         <v>8234</v>
@@ -2214,13 +2216,13 @@
         <v>16038</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E40" s="15" t="n">
         <v>7832</v>
@@ -2235,13 +2237,13 @@
         <v>16039</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E41" s="15" t="n">
         <v>4179</v>
@@ -2256,13 +2258,13 @@
         <v>16040</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E42" s="15" t="n">
         <v>5901</v>
@@ -2277,13 +2279,13 @@
         <v>16041</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E43" s="15" t="n">
         <v>95</v>
@@ -2298,13 +2300,13 @@
         <v>16042</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E44" s="15" t="n">
         <v>5354</v>
@@ -2319,13 +2321,13 @@
         <v>16043</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E45" s="15" t="n">
         <v>5878</v>
@@ -2340,13 +2342,13 @@
         <v>16044</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E46" s="15" t="n">
         <v>5410</v>
@@ -2361,13 +2363,13 @@
         <v>16046</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E47" s="15" t="n">
         <v>8342</v>
@@ -2382,13 +2384,13 @@
         <v>16047</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E48" s="15" t="n">
         <v>4030</v>
@@ -2412,13 +2414,13 @@
         <v>16048</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E49" s="15" t="n">
         <v>619</v>
@@ -2442,13 +2444,13 @@
         <v>16049</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E50" s="15" t="n">
         <v>4455</v>
@@ -2463,13 +2465,13 @@
         <v>16050</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E51" s="15" t="n">
         <v>1347</v>
@@ -2484,13 +2486,13 @@
         <v>16051</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E52" s="15" t="n">
         <v>7819</v>
@@ -2505,13 +2507,13 @@
         <v>16052</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E53" s="15" t="n">
         <v>3120</v>
@@ -2526,13 +2528,13 @@
         <v>16053</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E54" s="15" t="n">
         <v>16228</v>
@@ -2556,13 +2558,13 @@
         <v>16055</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E55" s="15" t="n">
         <v>4619</v>
@@ -2586,13 +2588,13 @@
         <v>16056</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E56" s="15" t="n">
         <v>355</v>
@@ -2607,13 +2609,13 @@
         <v>16057</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E57" s="15" t="n">
         <v>4651</v>
@@ -2628,13 +2630,13 @@
         <v>16058</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E58" s="15" t="n">
         <v>4053</v>
@@ -2658,13 +2660,13 @@
         <v>16059</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E59" s="15" t="n">
         <v>3956</v>
@@ -2679,13 +2681,13 @@
         <v>16060</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E60" s="15" t="n">
         <v>3343</v>
@@ -2700,13 +2702,13 @@
         <v>16061</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E61" s="15" t="n">
         <v>120</v>
@@ -2721,13 +2723,13 @@
         <v>16063</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E62" s="15" t="n">
         <v>2918</v>
@@ -2751,13 +2753,13 @@
         <v>16062</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E63" s="15" t="n">
         <v>10016</v>
@@ -2781,13 +2783,13 @@
         <v>16064</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E64" s="15" t="n">
         <v>3476</v>
@@ -2811,13 +2813,13 @@
         <v>16065</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E65" s="15" t="n">
         <v>1438</v>
@@ -2832,13 +2834,13 @@
         <v>16066</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E66" s="15" t="n">
         <v>2450</v>
@@ -2862,13 +2864,13 @@
         <v>16067</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E67" s="15" t="n">
         <v>1604</v>
@@ -2883,13 +2885,13 @@
         <v>16068</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E68" s="15" t="n">
         <v>2524</v>
@@ -2904,13 +2906,13 @@
         <v>16069</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E69" s="15" t="n">
         <v>3463</v>
@@ -2925,13 +2927,13 @@
         <v>16070</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E70" s="15" t="n">
         <v>4225</v>
@@ -2946,13 +2948,13 @@
         <v>16071</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E71" s="15" t="n">
         <v>1669</v>
@@ -2976,13 +2978,13 @@
         <v>16072</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E72" s="15" t="n">
         <v>3239</v>
@@ -2997,13 +2999,13 @@
         <v>16073</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E73" s="15" t="n">
         <v>5861</v>
@@ -3018,13 +3020,13 @@
         <v>16074</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E74" s="15" t="n">
         <v>6316</v>
@@ -3039,13 +3041,13 @@
         <v>16075</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E75" s="15" t="n">
         <v>5769</v>
@@ -3069,13 +3071,13 @@
         <v>16076</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E76" s="15" t="n">
         <v>5194</v>
@@ -3090,13 +3092,13 @@
         <v>16077</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E77" s="15" t="n">
         <v>8793</v>
@@ -3120,13 +3122,13 @@
         <v>16078</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E78" s="15" t="n">
         <v>1141</v>
@@ -3141,13 +3143,13 @@
         <v>16079</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E79" s="15" t="n">
         <v>10759</v>
@@ -3171,13 +3173,13 @@
         <v>16080</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E80" s="15" t="n">
         <v>1674</v>
@@ -3192,13 +3194,13 @@
         <v>16081</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E81" s="15" t="n">
         <v>4144</v>
@@ -3213,13 +3215,13 @@
         <v>16082</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E82" s="15" t="n">
         <v>969</v>
@@ -3243,13 +3245,13 @@
         <v>16249</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E83" s="15" t="n">
         <v>310</v>
@@ -3264,13 +3266,13 @@
         <v>16083</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E84" s="15" t="n">
         <v>1959</v>
@@ -3285,13 +3287,13 @@
         <v>16084</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E85" s="15" t="n">
         <v>3369</v>
@@ -3306,13 +3308,13 @@
         <v>16247</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E86" s="15" t="n">
         <v>980</v>
@@ -3327,13 +3329,13 @@
         <v>16085</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E87" s="15" t="n">
         <v>624</v>
@@ -3348,13 +3350,13 @@
         <v>16086</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E88" s="15" t="n">
         <v>9333</v>
@@ -3369,13 +3371,13 @@
         <v>16087</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E89" s="15" t="n">
         <v>4140</v>
@@ -3399,13 +3401,13 @@
         <v>16088</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E90" s="15" t="n">
         <v>3400</v>
@@ -3420,13 +3422,13 @@
         <v>16089</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E91" s="15" t="n">
         <v>7752</v>
@@ -3450,13 +3452,13 @@
         <v>16090</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E92" s="15" t="n">
         <v>265</v>
@@ -3471,13 +3473,13 @@
         <v>16091</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E93" s="15" t="n">
         <v>23266</v>
@@ -3501,13 +3503,13 @@
         <v>16092</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E94" s="15" t="n">
         <v>966</v>
@@ -3531,13 +3533,13 @@
         <v>16093</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E95" s="15" t="n">
         <v>3553</v>
@@ -3561,13 +3563,13 @@
         <v>16094</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E96" s="15" t="n">
         <v>1887</v>
@@ -3582,13 +3584,13 @@
         <v>16096</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E97" s="15" t="n">
         <v>7970</v>
@@ -3603,13 +3605,13 @@
         <v>16097</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E98" s="15" t="n">
         <v>1329</v>
@@ -3624,13 +3626,13 @@
         <v>16098</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E99" s="15" t="n">
         <v>3224</v>
@@ -3645,13 +3647,13 @@
         <v>16099</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E100" s="15" t="n">
         <v>1153</v>
@@ -3666,13 +3668,13 @@
         <v>16100</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E101" s="15" t="n">
         <v>3097</v>
@@ -3687,13 +3689,13 @@
         <v>16101</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E102" s="15" t="n">
         <v>4339</v>
@@ -3708,13 +3710,13 @@
         <v>16102</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E103" s="15" t="n">
         <v>691</v>
@@ -3738,13 +3740,13 @@
         <v>16103</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E104" s="15" t="n">
         <v>206</v>
@@ -3768,13 +3770,13 @@
         <v>16104</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E105" s="15" t="n">
         <v>3151</v>
@@ -3789,13 +3791,13 @@
         <v>16105</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E106" s="15" t="n">
         <v>3305</v>
@@ -3810,13 +3812,13 @@
         <v>16106</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E107" s="15" t="n">
         <v>226</v>
@@ -3831,13 +3833,13 @@
         <v>16107</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E108" s="15" t="n">
         <v>1065</v>
@@ -3852,13 +3854,13 @@
         <v>16108</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D109" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E109" s="15" t="n">
         <v>5697</v>
@@ -3882,13 +3884,13 @@
         <v>16109</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D110" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E110" s="15" t="n">
         <v>1527</v>
@@ -3903,13 +3905,13 @@
         <v>16110</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D111" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E111" s="15" t="n">
         <v>931</v>
@@ -3924,13 +3926,13 @@
         <v>16111</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D112" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E112" s="15" t="n">
         <v>5161</v>
@@ -3954,13 +3956,13 @@
         <v>16112</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D113" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E113" s="15" t="n">
         <v>360</v>
@@ -3975,13 +3977,13 @@
         <v>16113</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D114" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E114" s="15" t="n">
         <v>5945</v>
@@ -3996,13 +3998,13 @@
         <v>16114</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D115" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E115" s="15" t="n">
         <v>5062</v>
@@ -4017,13 +4019,13 @@
         <v>16115</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D116" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E116" s="15" t="n">
         <v>6404</v>
@@ -4047,13 +4049,13 @@
         <v>16116</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C117" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E117" s="15" t="n">
         <v>1684</v>
@@ -4068,13 +4070,13 @@
         <v>16117</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D118" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E118" s="15" t="n">
         <v>6322</v>
@@ -4089,13 +4091,13 @@
         <v>16118</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D119" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E119" s="15" t="n">
         <v>1252</v>
@@ -4110,13 +4112,13 @@
         <v>16119</v>
       </c>
       <c r="B120" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D120" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E120" s="15" t="n">
         <v>934</v>
@@ -4131,13 +4133,13 @@
         <v>16120</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D121" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E121" s="15" t="n">
         <v>7360</v>
@@ -4152,13 +4154,13 @@
         <v>16121</v>
       </c>
       <c r="B122" s="14" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D122" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E122" s="15" t="n">
         <v>189</v>
@@ -4182,13 +4184,13 @@
         <v>16122</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D123" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E123" s="15" t="n">
         <v>664</v>
@@ -4203,13 +4205,13 @@
         <v>16123</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D124" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E124" s="15" t="n">
         <v>4138</v>
@@ -4224,13 +4226,13 @@
         <v>16124</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D125" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E125" s="15" t="n">
         <v>4730</v>
@@ -4245,13 +4247,13 @@
         <v>16125</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D126" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E126" s="15" t="n">
         <v>640</v>
@@ -4275,13 +4277,13 @@
         <v>16126</v>
       </c>
       <c r="B127" s="14" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D127" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E127" s="15" t="n">
         <v>3813</v>
@@ -4296,13 +4298,13 @@
         <v>16127</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D128" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E128" s="15" t="n">
         <v>853</v>
@@ -4326,13 +4328,13 @@
         <v>16128</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D129" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E129" s="15" t="n">
         <v>5428</v>
@@ -4347,13 +4349,13 @@
         <v>16129</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D130" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E130" s="15" t="n">
         <v>2566</v>
@@ -4368,13 +4370,13 @@
         <v>16130</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D131" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E131" s="15" t="n">
         <v>868</v>
@@ -4389,13 +4391,13 @@
         <v>16131</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D132" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E132" s="15" t="n">
         <v>4031</v>
@@ -4410,13 +4412,13 @@
         <v>16132</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D133" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E133" s="15" t="n">
         <v>6446</v>
@@ -4440,13 +4442,13 @@
         <v>16133</v>
       </c>
       <c r="B134" s="14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C134" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D134" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E134" s="15" t="n">
         <v>10121</v>
@@ -4470,13 +4472,13 @@
         <v>16250</v>
       </c>
       <c r="B135" s="14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C135" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D135" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E135" s="15" t="n">
         <v>2388</v>
@@ -4491,13 +4493,13 @@
         <v>16134</v>
       </c>
       <c r="B136" s="14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D136" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E136" s="15" t="n">
         <v>196</v>
@@ -4512,13 +4514,13 @@
         <v>16135</v>
       </c>
       <c r="B137" s="14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C137" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D137" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E137" s="15" t="n">
         <v>2986</v>
@@ -4533,13 +4535,13 @@
         <v>16136</v>
       </c>
       <c r="B138" s="14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C138" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D138" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E138" s="15" t="n">
         <v>208</v>
@@ -4554,13 +4556,13 @@
         <v>16137</v>
       </c>
       <c r="B139" s="14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C139" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D139" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E139" s="15" t="n">
         <v>1119</v>
@@ -4575,13 +4577,13 @@
         <v>16139</v>
       </c>
       <c r="B140" s="14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C140" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D140" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E140" s="15" t="n">
         <v>3253</v>
@@ -4596,13 +4598,13 @@
         <v>16140</v>
       </c>
       <c r="B141" s="14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C141" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D141" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E141" s="15" t="n">
         <v>2600</v>
@@ -4617,13 +4619,13 @@
         <v>16141</v>
       </c>
       <c r="B142" s="14" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C142" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D142" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E142" s="15" t="n">
         <v>2897</v>
@@ -4638,13 +4640,13 @@
         <v>16142</v>
       </c>
       <c r="B143" s="14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C143" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D143" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E143" s="15" t="n">
         <v>4619</v>
@@ -4659,13 +4661,13 @@
         <v>16143</v>
       </c>
       <c r="B144" s="14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C144" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D144" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E144" s="15" t="n">
         <v>7488</v>
@@ -4689,13 +4691,13 @@
         <v>16144</v>
       </c>
       <c r="B145" s="14" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C145" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D145" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E145" s="15" t="n">
         <v>11636</v>
@@ -4719,13 +4721,13 @@
         <v>16145</v>
       </c>
       <c r="B146" s="14" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C146" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D146" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E146" s="15" t="n">
         <v>525</v>
@@ -4740,13 +4742,13 @@
         <v>16146</v>
       </c>
       <c r="B147" s="14" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C147" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D147" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E147" s="15" t="n">
         <v>1062</v>
@@ -4761,13 +4763,13 @@
         <v>16147</v>
       </c>
       <c r="B148" s="14" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C148" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D148" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E148" s="15" t="n">
         <v>186</v>
@@ -4782,13 +4784,13 @@
         <v>16148</v>
       </c>
       <c r="B149" s="14" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C149" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D149" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E149" s="15" t="n">
         <v>661</v>
@@ -4803,13 +4805,13 @@
         <v>16149</v>
       </c>
       <c r="B150" s="14" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C150" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D150" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E150" s="15" t="n">
         <v>835</v>
@@ -4833,13 +4835,13 @@
         <v>16150</v>
       </c>
       <c r="B151" s="14" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C151" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D151" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E151" s="15" t="n">
         <v>1752</v>
@@ -4863,13 +4865,13 @@
         <v>16151</v>
       </c>
       <c r="B152" s="14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C152" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D152" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E152" s="15" t="n">
         <v>180</v>
@@ -4884,13 +4886,13 @@
         <v>16152</v>
       </c>
       <c r="B153" s="14" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C153" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D153" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E153" s="15" t="n">
         <v>5115</v>
@@ -4905,13 +4907,13 @@
         <v>16153</v>
       </c>
       <c r="B154" s="14" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C154" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D154" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E154" s="15" t="n">
         <v>11890</v>
@@ -4935,13 +4937,13 @@
         <v>16154</v>
       </c>
       <c r="B155" s="14" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C155" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D155" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E155" s="15" t="n">
         <v>2103</v>
@@ -4956,13 +4958,13 @@
         <v>16155</v>
       </c>
       <c r="B156" s="14" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D156" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E156" s="15" t="n">
         <v>4002</v>
@@ -4986,13 +4988,13 @@
         <v>16156</v>
       </c>
       <c r="B157" s="14" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D157" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E157" s="15" t="n">
         <v>4215</v>
@@ -5007,13 +5009,13 @@
         <v>16157</v>
       </c>
       <c r="B158" s="14" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D158" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E158" s="15" t="n">
         <v>5801</v>
@@ -5028,13 +5030,13 @@
         <v>16158</v>
       </c>
       <c r="B159" s="14" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D159" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E159" s="15" t="n">
         <v>2815</v>
@@ -5049,13 +5051,13 @@
         <v>16159</v>
       </c>
       <c r="B160" s="14" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D160" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E160" s="15" t="n">
         <v>375</v>
@@ -5070,13 +5072,13 @@
         <v>16160</v>
       </c>
       <c r="B161" s="14" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C161" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D161" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E161" s="15" t="n">
         <v>5777</v>
@@ -5091,13 +5093,13 @@
         <v>16161</v>
       </c>
       <c r="B162" s="14" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C162" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D162" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E162" s="15" t="n">
         <v>1857</v>
@@ -5112,13 +5114,13 @@
         <v>16162</v>
       </c>
       <c r="B163" s="14" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C163" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D163" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E163" s="15" t="n">
         <v>1544</v>
@@ -5133,13 +5135,13 @@
         <v>16163</v>
       </c>
       <c r="B164" s="14" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C164" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D164" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E164" s="15" t="n">
         <v>1106</v>
@@ -5154,13 +5156,13 @@
         <v>16164</v>
       </c>
       <c r="B165" s="14" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C165" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D165" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E165" s="15" t="n">
         <v>1256</v>
@@ -5175,13 +5177,13 @@
         <v>16165</v>
       </c>
       <c r="B166" s="14" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C166" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D166" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E166" s="15" t="n">
         <v>444</v>
@@ -5196,13 +5198,13 @@
         <v>16166</v>
       </c>
       <c r="B167" s="14" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C167" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D167" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E167" s="15" t="n">
         <v>86</v>
@@ -5226,13 +5228,13 @@
         <v>16167</v>
       </c>
       <c r="B168" s="14" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C168" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D168" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E168" s="15" t="n">
         <v>1571</v>
@@ -5247,13 +5249,13 @@
         <v>16168</v>
       </c>
       <c r="B169" s="14" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C169" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D169" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E169" s="15" t="n">
         <v>1923</v>
@@ -5268,13 +5270,13 @@
         <v>16170</v>
       </c>
       <c r="B170" s="14" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C170" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D170" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E170" s="15" t="n">
         <v>11543</v>
@@ -5298,13 +5300,13 @@
         <v>16169</v>
       </c>
       <c r="B171" s="14" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C171" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D171" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E171" s="15" t="n">
         <v>6825</v>
@@ -5328,13 +5330,13 @@
         <v>16171</v>
       </c>
       <c r="B172" s="14" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C172" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D172" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E172" s="15" t="n">
         <v>3229</v>
@@ -5349,13 +5351,13 @@
         <v>16172</v>
       </c>
       <c r="B173" s="14" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C173" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D173" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E173" s="15" t="n">
         <v>5102</v>
@@ -5379,13 +5381,13 @@
         <v>16173</v>
       </c>
       <c r="B174" s="14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C174" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D174" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E174" s="15" t="n">
         <v>4593</v>
@@ -5409,13 +5411,13 @@
         <v>16174</v>
       </c>
       <c r="B175" s="14" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C175" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D175" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E175" s="15" t="n">
         <v>1895</v>
@@ -5430,13 +5432,13 @@
         <v>16175</v>
       </c>
       <c r="B176" s="14" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C176" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D176" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E176" s="15" t="n">
         <v>1166</v>
@@ -5451,13 +5453,13 @@
         <v>16176</v>
       </c>
       <c r="B177" s="14" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C177" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D177" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E177" s="15" t="n">
         <v>4896</v>
@@ -5472,13 +5474,13 @@
         <v>16177</v>
       </c>
       <c r="B178" s="14" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C178" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D178" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E178" s="15" t="n">
         <v>1694</v>
@@ -5493,13 +5495,13 @@
         <v>16178</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C179" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D179" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E179" s="15" t="n">
         <v>6018</v>
@@ -5523,13 +5525,13 @@
         <v>16179</v>
       </c>
       <c r="B180" s="14" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C180" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D180" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E180" s="15" t="n">
         <v>1310</v>
@@ -5544,13 +5546,13 @@
         <v>16180</v>
       </c>
       <c r="B181" s="14" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C181" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D181" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E181" s="15" t="n">
         <v>867</v>
@@ -5574,13 +5576,13 @@
         <v>16182</v>
       </c>
       <c r="B182" s="14" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C182" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D182" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E182" s="15" t="n">
         <v>3966</v>
@@ -5595,13 +5597,13 @@
         <v>16183</v>
       </c>
       <c r="B183" s="14" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C183" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D183" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E183" s="15" t="n">
         <v>19049</v>
@@ -5625,13 +5627,13 @@
         <v>16184</v>
       </c>
       <c r="B184" s="14" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C184" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D184" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E184" s="15" t="n">
         <v>436</v>
@@ -5655,13 +5657,13 @@
         <v>16185</v>
       </c>
       <c r="B185" s="14" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C185" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D185" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E185" s="15" t="n">
         <v>754</v>
@@ -5676,13 +5678,13 @@
         <v>16186</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C186" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D186" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E186" s="15" t="n">
         <v>924</v>
@@ -5697,13 +5699,13 @@
         <v>16187</v>
       </c>
       <c r="B187" s="14" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C187" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D187" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E187" s="15" t="n">
         <v>3966</v>
@@ -5718,13 +5720,13 @@
         <v>16188</v>
       </c>
       <c r="B188" s="14" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C188" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D188" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E188" s="15" t="n">
         <v>5094</v>
@@ -5748,13 +5750,13 @@
         <v>16189</v>
       </c>
       <c r="B189" s="14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C189" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D189" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E189" s="15" t="n">
         <v>5435</v>
@@ -5769,13 +5771,13 @@
         <v>16190</v>
       </c>
       <c r="B190" s="14" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C190" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D190" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E190" s="15" t="n">
         <v>4974</v>
@@ -5799,13 +5801,13 @@
         <v>16191</v>
       </c>
       <c r="B191" s="14" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C191" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D191" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E191" s="15" t="n">
         <v>586</v>
@@ -5829,13 +5831,13 @@
         <v>16192</v>
       </c>
       <c r="B192" s="14" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C192" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D192" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E192" s="15" t="n">
         <v>3571</v>
@@ -5850,13 +5852,13 @@
         <v>16193</v>
       </c>
       <c r="B193" s="14" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C193" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D193" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E193" s="15" t="n">
         <v>6652</v>
@@ -5871,13 +5873,13 @@
         <v>16194</v>
       </c>
       <c r="B194" s="14" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C194" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D194" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E194" s="15" t="n">
         <v>9843</v>
@@ -5901,13 +5903,13 @@
         <v>16195</v>
       </c>
       <c r="B195" s="14" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C195" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D195" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E195" s="15" t="n">
         <v>1265</v>
@@ -5931,13 +5933,13 @@
         <v>16196</v>
       </c>
       <c r="B196" s="14" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C196" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D196" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E196" s="15" t="n">
         <v>2559</v>
@@ -5961,13 +5963,13 @@
         <v>16197</v>
       </c>
       <c r="B197" s="14" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C197" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D197" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E197" s="15" t="n">
         <v>2015</v>
@@ -5991,13 +5993,13 @@
         <v>16198</v>
       </c>
       <c r="B198" s="14" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C198" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D198" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E198" s="15" t="n">
         <v>24297</v>
@@ -6021,13 +6023,13 @@
         <v>16199</v>
       </c>
       <c r="B199" s="14" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C199" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D199" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E199" s="15" t="n">
         <v>2187</v>
@@ -6051,13 +6053,13 @@
         <v>16200</v>
       </c>
       <c r="B200" s="14" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C200" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D200" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E200" s="15" t="n">
         <v>1709</v>
@@ -6072,13 +6074,13 @@
         <v>16251</v>
       </c>
       <c r="B201" s="14" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C201" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D201" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E201" s="15" t="n">
         <v>1948</v>
@@ -6093,13 +6095,13 @@
         <v>16201</v>
       </c>
       <c r="B202" s="14" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C202" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D202" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E202" s="15" t="n">
         <v>701</v>
@@ -6123,13 +6125,13 @@
         <v>16202</v>
       </c>
       <c r="B203" s="14" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C203" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D203" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E203" s="15" t="n">
         <v>9120</v>
@@ -6144,13 +6146,13 @@
         <v>16203</v>
       </c>
       <c r="B204" s="14" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C204" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D204" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E204" s="15" t="n">
         <v>4239</v>
@@ -6165,13 +6167,13 @@
         <v>16204</v>
       </c>
       <c r="B205" s="14" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C205" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D205" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E205" s="15" t="n">
         <v>5486</v>
@@ -6186,13 +6188,13 @@
         <v>16205</v>
       </c>
       <c r="B206" s="14" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C206" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D206" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E206" s="15" t="n">
         <v>1037</v>
@@ -6207,13 +6209,13 @@
         <v>16206</v>
       </c>
       <c r="B207" s="14" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C207" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D207" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E207" s="15" t="n">
         <v>5652</v>
@@ -6237,13 +6239,13 @@
         <v>16207</v>
       </c>
       <c r="B208" s="14" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C208" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D208" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E208" s="15" t="n">
         <v>12867</v>
@@ -6267,13 +6269,13 @@
         <v>16208</v>
       </c>
       <c r="B209" s="14" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C209" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D209" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E209" s="15" t="n">
         <v>1075</v>
@@ -6288,13 +6290,13 @@
         <v>16209</v>
       </c>
       <c r="B210" s="14" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C210" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D210" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E210" s="15" t="n">
         <v>3888</v>
@@ -6309,13 +6311,13 @@
         <v>16210</v>
       </c>
       <c r="B211" s="14" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C211" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D211" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E211" s="15" t="n">
         <v>625</v>
@@ -6330,13 +6332,13 @@
         <v>16211</v>
       </c>
       <c r="B212" s="14" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C212" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D212" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E212" s="15" t="n">
         <v>2146</v>
@@ -6351,13 +6353,13 @@
         <v>16212</v>
       </c>
       <c r="B213" s="14" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C213" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D213" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E213" s="15" t="n">
         <v>4847</v>
@@ -6381,13 +6383,13 @@
         <v>16213</v>
       </c>
       <c r="B214" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C214" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D214" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E214" s="15" t="n">
         <v>7665</v>
@@ -6402,13 +6404,13 @@
         <v>16214</v>
       </c>
       <c r="B215" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C215" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D215" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E215" s="15" t="n">
         <v>8334</v>
@@ -6432,13 +6434,13 @@
         <v>16216</v>
       </c>
       <c r="B216" s="14" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C216" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D216" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E216" s="15" t="n">
         <v>2326</v>
@@ -6453,13 +6455,13 @@
         <v>16217</v>
       </c>
       <c r="B217" s="14" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C217" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D217" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E217" s="15" t="n">
         <v>1138</v>
@@ -6474,13 +6476,13 @@
         <v>16218</v>
       </c>
       <c r="B218" s="14" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C218" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D218" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E218" s="15" t="n">
         <v>9685</v>
@@ -6495,13 +6497,13 @@
         <v>16219</v>
       </c>
       <c r="B219" s="14" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C219" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D219" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E219" s="15" t="n">
         <v>29034</v>
@@ -6525,13 +6527,13 @@
         <v>16220</v>
       </c>
       <c r="B220" s="14" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C220" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D220" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E220" s="15" t="n">
         <v>10297</v>
@@ -6555,13 +6557,13 @@
         <v>16221</v>
       </c>
       <c r="B221" s="14" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C221" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D221" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E221" s="15" t="n">
         <v>1395</v>
@@ -6585,13 +6587,13 @@
         <v>16222</v>
       </c>
       <c r="B222" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C222" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D222" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E222" s="15" t="n">
         <v>9592</v>
@@ -6606,13 +6608,13 @@
         <v>16223</v>
       </c>
       <c r="B223" s="14" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C223" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D223" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E223" s="15" t="n">
         <v>1097</v>
@@ -6636,13 +6638,13 @@
         <v>16224</v>
       </c>
       <c r="B224" s="14" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C224" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D224" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E224" s="15" t="n">
         <v>3753</v>
@@ -6657,13 +6659,13 @@
         <v>16225</v>
       </c>
       <c r="B225" s="14" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C225" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D225" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E225" s="15" t="n">
         <v>616</v>
@@ -6678,13 +6680,13 @@
         <v>16226</v>
       </c>
       <c r="B226" s="14" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C226" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D226" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E226" s="15" t="n">
         <v>137</v>
@@ -6699,13 +6701,13 @@
         <v>16227</v>
       </c>
       <c r="B227" s="14" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C227" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D227" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E227" s="15" t="n">
         <v>209</v>
@@ -6729,13 +6731,13 @@
         <v>16228</v>
       </c>
       <c r="B228" s="14" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C228" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D228" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E228" s="15" t="n">
         <v>425</v>
@@ -6750,13 +6752,13 @@
         <v>16229</v>
       </c>
       <c r="B229" s="14" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C229" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D229" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E229" s="15" t="n">
         <v>295</v>
@@ -6771,13 +6773,13 @@
         <v>16230</v>
       </c>
       <c r="B230" s="14" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C230" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D230" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E230" s="15" t="n">
         <v>217</v>
@@ -6792,13 +6794,13 @@
         <v>16232</v>
       </c>
       <c r="B231" s="14" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C231" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D231" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E231" s="15" t="n">
         <v>7790</v>
@@ -6813,13 +6815,13 @@
         <v>16233</v>
       </c>
       <c r="B232" s="14" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C232" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D232" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E232" s="15" t="n">
         <v>7829</v>
@@ -6834,13 +6836,13 @@
         <v>16234</v>
       </c>
       <c r="B233" s="14" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C233" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D233" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E233" s="15" t="n">
         <v>4871</v>
@@ -6855,13 +6857,13 @@
         <v>16235</v>
       </c>
       <c r="B234" s="14" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C234" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D234" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E234" s="15" t="n">
         <v>1142</v>
@@ -6876,13 +6878,13 @@
         <v>16236</v>
       </c>
       <c r="B235" s="14" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C235" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D235" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E235" s="15" t="n">
         <v>1260</v>
@@ -6897,13 +6899,13 @@
         <v>16237</v>
       </c>
       <c r="B236" s="14" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C236" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D236" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E236" s="15" t="n">
         <v>603</v>
@@ -6927,13 +6929,13 @@
         <v>16238</v>
       </c>
       <c r="B237" s="14" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C237" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D237" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E237" s="15" t="n">
         <v>4729</v>
@@ -6948,13 +6950,13 @@
         <v>16239</v>
       </c>
       <c r="B238" s="14" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C238" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D238" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E238" s="15" t="n">
         <v>6844</v>
@@ -6969,13 +6971,13 @@
         <v>16240</v>
       </c>
       <c r="B239" s="14" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C239" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D239" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E239" s="15" t="n">
         <v>6608</v>
@@ -6990,13 +6992,13 @@
         <v>16241</v>
       </c>
       <c r="B240" s="14" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C240" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D240" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E240" s="15" t="n">
         <v>1982</v>
@@ -7011,13 +7013,13 @@
         <v>16242</v>
       </c>
       <c r="B241" s="14" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C241" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D241" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E241" s="15" t="n">
         <v>7770</v>
@@ -7041,13 +7043,13 @@
         <v>16243</v>
       </c>
       <c r="B242" s="14" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C242" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D242" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E242" s="15" t="n">
         <v>1532</v>
@@ -7071,13 +7073,13 @@
         <v>16244</v>
       </c>
       <c r="B243" s="14" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C243" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D243" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E243" s="15" t="n">
         <v>2746</v>
@@ -7092,13 +7094,13 @@
         <v>16245</v>
       </c>
       <c r="B244" s="14" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C244" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D244" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E244" s="15" t="n">
         <v>8190</v>
@@ -7113,13 +7115,13 @@
         <v>16246</v>
       </c>
       <c r="B245" s="14" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C245" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D245" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E245" s="15" t="n">
         <v>9097</v>

</xml_diff>

<commit_message>
final data march 2020
</commit_message>
<xml_diff>
--- a/opendata/it-bergamo-deaths-03.xlsx
+++ b/opendata/it-bergamo-deaths-03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Riassunto Bergamo" sheetId="1" state="visible" r:id="rId2"/>
@@ -834,12 +834,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
-    <numFmt numFmtId="167" formatCode="YYYY\-MM"/>
-    <numFmt numFmtId="168" formatCode="General"/>
+    <numFmt numFmtId="167" formatCode="0"/>
+    <numFmt numFmtId="168" formatCode="YYYY\-MM"/>
+    <numFmt numFmtId="169" formatCode="General"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -959,7 +960,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1000,7 +1001,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1008,11 +1009,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1020,15 +1021,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1063,7 +1068,7 @@
   </sheetPr>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1233,16 +1238,16 @@
   </sheetPr>
   <dimension ref="A1:AMJ247"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="11.11"/>
@@ -7145,19 +7150,19 @@
         <f aca="false">SUM(E2:E245)</f>
         <v>1098740</v>
       </c>
-      <c r="F247" s="18" t="n">
+      <c r="F247" s="19" t="n">
         <f aca="false">SUM(F2:F245)</f>
         <v>499</v>
       </c>
-      <c r="G247" s="18" t="n">
+      <c r="G247" s="19" t="n">
         <f aca="false">SUM(G2:G245)</f>
         <v>2917</v>
       </c>
-      <c r="H247" s="18" t="n">
+      <c r="H247" s="19" t="n">
         <f aca="false">SUM(H2:H245)</f>
         <v>1140</v>
       </c>
-      <c r="I247" s="19" t="n">
+      <c r="I247" s="20" t="n">
         <f aca="false">SUM(I2:I245)</f>
         <v>573809</v>
       </c>

</xml_diff>